<commit_message>
updated testing files and removed accidental debug.writeline left in
</commit_message>
<xml_diff>
--- a/TextReplace.Tests/MockFiles/OutputTests/Outputs/CaseSensitive/output-financial-sample-case-sensitive.xlsx
+++ b/TextReplace.Tests/MockFiles/OutputTests/Outputs/CaseSensitive/output-financial-sample-case-sensitive.xlsx
@@ -527,28 +527,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="financials" displayName="financials" ref="A1:P701" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowCellStyle="Currency" dataCellStyle="Currency">
-  <autoFilter ref="A1:P701"/>
-  <tableColumns count="16">
-    <tableColumn id="1" name="Segment"/>
-    <tableColumn id="2" name="Country"/>
-    <tableColumn id="16" name="Product" dataDxfId="12" dataCellStyle="Currency"/>
-    <tableColumn id="19" name="Discount Band" dataDxfId="11" dataCellStyle="Currency"/>
-    <tableColumn id="6" name="Units Sold"/>
-    <tableColumn id="7" name="Manufacturing Price" dataDxfId="10" dataCellStyle="Currency"/>
-    <tableColumn id="8" name="Sale Price" dataDxfId="9" dataCellStyle="Currency"/>
-    <tableColumn id="9" name="Gross Sales" dataDxfId="8" dataCellStyle="Currency"/>
-    <tableColumn id="10" name="Discounts" dataDxfId="7" dataCellStyle="Currency"/>
-    <tableColumn id="11" name=" Sales" dataDxfId="6" dataCellStyle="Currency"/>
-    <tableColumn id="12" name="COGS" dataDxfId="5" dataCellStyle="Currency"/>
-    <tableColumn id="13" name="Profit" dataDxfId="4" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="Date" dataDxfId="3" dataCellStyle="Currency"/>
-    <tableColumn id="17" name="Month Number" dataDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="18" name="Month Name" dataDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="20" name="Year" dataDxfId="0" dataCellStyle="Currency"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="financials" displayName="financials" ref="A1:P701" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowCellStyle="Currency" dataCellStyle="Currency">
+  <x:autoFilter ref="A1:P701"/>
+  <x:tableColumns count="16">
+    <x:tableColumn id="1" name="Segment"/>
+    <x:tableColumn id="2" name="Country"/>
+    <x:tableColumn id="16" name="Product" dataDxfId="12" dataCellStyle="Currency"/>
+    <x:tableColumn id="19" name="Discount Band" dataDxfId="11" dataCellStyle="Currency"/>
+    <x:tableColumn id="6" name="Units Sold"/>
+    <x:tableColumn id="7" name="Mfg Price" dataDxfId="10" dataCellStyle="Currency"/>
+    <x:tableColumn id="8" name="Sale Price" dataDxfId="9" dataCellStyle="Currency"/>
+    <x:tableColumn id="9" name="Gross Sales" dataDxfId="8" dataCellStyle="Currency"/>
+    <x:tableColumn id="10" name="Discounts" dataDxfId="7" dataCellStyle="Currency"/>
+    <x:tableColumn id="11" name=" Sales" dataDxfId="6" dataCellStyle="Currency"/>
+    <x:tableColumn id="12" name="COGS" dataDxfId="5" dataCellStyle="Currency"/>
+    <x:tableColumn id="13" name="Profit" dataDxfId="4" dataCellStyle="Currency"/>
+    <x:tableColumn id="4" name="Date" dataDxfId="3" dataCellStyle="Currency"/>
+    <x:tableColumn id="17" name="Month Number" dataDxfId="2" dataCellStyle="Currency"/>
+    <x:tableColumn id="18" name="Month Name" dataDxfId="1" dataCellStyle="Currency"/>
+    <x:tableColumn id="20" name="Yr" dataDxfId="0" dataCellStyle="Currency"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>